<commit_message>
23-10-2024 – Designing Database
</commit_message>
<xml_diff>
--- a/.tmp/perancangan_website_sekolah.xlsx
+++ b/.tmp/perancangan_website_sekolah.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="V:\User\Documents\Project\website-sekolah\.tmp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D369FF15-857E-4B39-964B-D5595D8D2038}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B37E671-BEFA-4E88-B2F4-64421FAF3C9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11190" xr2:uid="{F4FE0CDE-66EF-46A1-87B3-9F6C6A79C11E}"/>
   </bookViews>
@@ -137,9 +137,6 @@
     <t>Komentar</t>
   </si>
   <si>
-    <t>GUID</t>
-  </si>
-  <si>
     <t>Name</t>
   </si>
   <si>
@@ -243,19 +240,28 @@
   </si>
   <si>
     <t>List Komentar (ID)</t>
+  </si>
+  <si>
+    <t>UUID</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
@@ -284,8 +290,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -637,8 +644,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3BC90C69-8BA9-4152-A242-BBA22C27B546}">
   <dimension ref="B2:I28"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.25" x14ac:dyDescent="0.25"/>
@@ -688,7 +695,7 @@
         <v>18</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="6" spans="2:9" x14ac:dyDescent="0.25">
@@ -705,7 +712,7 @@
         <v>16</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="7" spans="2:9" x14ac:dyDescent="0.25">
@@ -719,10 +726,10 @@
         <v>13</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="8" spans="2:9" x14ac:dyDescent="0.25">
@@ -738,7 +745,7 @@
     </row>
     <row r="10" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B10" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="12" spans="2:9" x14ac:dyDescent="0.25">
@@ -755,10 +762,10 @@
         <v>5</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="H12" s="1" t="s">
         <v>20</v>
@@ -766,25 +773,25 @@
     </row>
     <row r="13" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B13" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>27</v>
+        <v>54</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>62</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="14" spans="2:9" x14ac:dyDescent="0.25">
@@ -798,16 +805,16 @@
         <v>22</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="15" spans="2:9" x14ac:dyDescent="0.25">
@@ -821,16 +828,16 @@
         <v>23</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="16" spans="2:9" x14ac:dyDescent="0.25">
@@ -838,19 +845,19 @@
         <v>24</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.25">
@@ -858,24 +865,24 @@
         <v>22</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B18" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="19" spans="2:7" x14ac:dyDescent="0.25">
@@ -883,70 +890,70 @@
         <v>25</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>50</v>
+        <v>39</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>40</v>
+        <v>49</v>
       </c>
     </row>
     <row r="20" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B20" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="21" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B21" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>51</v>
+        <v>41</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>42</v>
+        <v>50</v>
       </c>
     </row>
     <row r="22" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B22" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="G22" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="23" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="F23" s="1" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="23" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="G23" s="1" t="s">
+    <row r="24" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="F24" s="1" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="24" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="G24" s="1" t="s">
+    <row r="25" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="F25" s="1" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="25" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="G25" s="1" t="s">
+    <row r="26" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="F26" s="1" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="26" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="G26" s="1" t="s">
+    <row r="27" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="F27" s="1" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="27" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="G27" s="1" t="s">
-        <v>48</v>
-      </c>
-    </row>
     <row r="28" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="G28" s="1" t="s">
-        <v>51</v>
+      <c r="F28" s="1" t="s">
+        <v>50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
25-10-2024 − Completing database structure
</commit_message>
<xml_diff>
--- a/.tmp/perancangan_website_sekolah.xlsx
+++ b/.tmp/perancangan_website_sekolah.xlsx
@@ -8,15 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="V:\User\Documents\Project\website-sekolah\.tmp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B37E671-BEFA-4E88-B2F4-64421FAF3C9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E07B4F0-E72B-47F6-8942-619A2B29DBCA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11190" xr2:uid="{F4FE0CDE-66EF-46A1-87B3-9F6C6A79C11E}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{F4FE0CDE-66EF-46A1-87B3-9F6C6A79C11E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
@@ -249,7 +252,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -645,34 +648,34 @@
   <dimension ref="B2:I28"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.25" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="3.28515625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="19.5703125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="20.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="20.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="3.25" style="1" customWidth="1"/>
+    <col min="2" max="2" width="19.625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="20.125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.375" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.375" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="20.875" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="9.125" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:9">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:9">
       <c r="B4" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:9">
       <c r="B5" s="1" t="s">
         <v>6</v>
       </c>
@@ -698,7 +701,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:9">
       <c r="B6" s="1" t="s">
         <v>7</v>
       </c>
@@ -715,7 +718,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:9">
       <c r="B7" s="1" t="s">
         <v>8</v>
       </c>
@@ -732,7 +735,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:9">
       <c r="B8" s="1" t="s">
         <v>9</v>
       </c>
@@ -743,12 +746,12 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:9">
       <c r="B10" s="1" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="12" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:9">
       <c r="B12" s="1" t="s">
         <v>19</v>
       </c>
@@ -771,7 +774,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:9">
       <c r="B13" s="1" t="s">
         <v>54</v>
       </c>
@@ -794,7 +797,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="14" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:9">
       <c r="B14" s="1" t="s">
         <v>21</v>
       </c>
@@ -817,7 +820,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="15" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:9">
       <c r="B15" s="1" t="s">
         <v>23</v>
       </c>
@@ -840,7 +843,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="16" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:9">
       <c r="B16" s="1" t="s">
         <v>24</v>
       </c>
@@ -860,7 +863,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:7">
       <c r="B17" s="1" t="s">
         <v>22</v>
       </c>
@@ -874,7 +877,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:7">
       <c r="B18" s="1" t="s">
         <v>28</v>
       </c>
@@ -885,7 +888,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:7">
       <c r="B19" s="1" t="s">
         <v>25</v>
       </c>
@@ -896,7 +899,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:7">
       <c r="B20" s="1" t="s">
         <v>55</v>
       </c>
@@ -907,7 +910,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:7">
       <c r="B21" s="1" t="s">
         <v>56</v>
       </c>
@@ -918,7 +921,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:7">
       <c r="B22" s="1" t="s">
         <v>61</v>
       </c>
@@ -926,32 +929,32 @@
         <v>42</v>
       </c>
     </row>
-    <row r="23" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:7">
       <c r="F23" s="1" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="24" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:7">
       <c r="F24" s="1" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="25" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:7">
       <c r="F25" s="1" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="26" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:7">
       <c r="F26" s="1" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="27" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:7">
       <c r="F27" s="1" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="28" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:7">
       <c r="F28" s="1" t="s">
         <v>50</v>
       </c>

</xml_diff>